<commit_message>
Unittests fuer 'insert_neuer_mitarbeiter' geschrieben.
</commit_message>
<xml_diff>
--- a/src/main/insert personenbezogene Daten/10 Mitarbeiter.xlsx
+++ b/src/main/insert personenbezogene Daten/10 Mitarbeiter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert personenbezogene Daten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FCB092-252D-4227-BD35-8AC6E6CA9865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D80270-5D81-4AE6-9553-16A2032F056C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5076" yWindow="2628" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -169,9 +169,6 @@
     <t>weiblich</t>
   </si>
   <si>
-    <t>Werkstudent</t>
-  </si>
-  <si>
     <t>Führungskraft</t>
   </si>
   <si>
@@ -187,15 +184,6 @@
     <t>Angestellter</t>
   </si>
   <si>
-    <t>Arbeiter</t>
-  </si>
-  <si>
-    <t>Auszubildender</t>
-  </si>
-  <si>
-    <t>Praktikant</t>
-  </si>
-  <si>
     <t>ja</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
   </si>
   <si>
     <t>ja/nein</t>
-  </si>
-  <si>
-    <t>Dualstudent</t>
   </si>
   <si>
     <t>A5-1</t>
@@ -402,25 +387,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -507,7 +474,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7DC797-A95E-4482-8629-011774679158}" name="tbl_Geschlecht" displayName="tbl_Geschlecht" ref="A1:A4" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C7DC797-A95E-4482-8629-011774679158}" name="tbl_Geschlecht" displayName="tbl_Geschlecht" ref="A1:A4" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:A4" xr:uid="{9C7DC797-A95E-4482-8629-011774679158}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F034D9B6-9D52-4274-B434-95E641979361}" name="Geschlecht"/>
@@ -517,18 +484,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D5ADE14-5AA7-4843-AE3B-15AFAD66EC57}" name="tbl_Mitarbeitertyp" displayName="tbl_Mitarbeitertyp" ref="C1:C7" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="C1:C7" xr:uid="{3D5ADE14-5AA7-4843-AE3B-15AFAD66EC57}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FCF90F50-8B26-48B9-9CDC-1309BA948D07}" name="Mitarbeitertyp"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}" name="tbl_Steuerklasse" displayName="tbl_Steuerklasse" ref="E1:E7" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="E1:E7" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}" name="tbl_Steuerklasse" displayName="tbl_Steuerklasse" ref="C1:C7" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="C1:C7" xr:uid="{5720A5BB-2C5B-4A43-93CC-F04ADFC83CAE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{51567C66-ECAC-455D-9A22-13EAF994E51B}" name="Steuerklasse"/>
   </tableColumns>
@@ -536,9 +493,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}" name="tbl_ja_nein" displayName="tbl_ja_nein" ref="G1:G3" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="G1:G3" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}" name="tbl_ja_nein" displayName="tbl_ja_nein" ref="E1:E3" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="E1:E3" xr:uid="{F422A189-5D14-462B-BE76-5CC30C61C2C5}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E96CACD0-03BA-4687-8818-6C96395A421D}" name="ja/nein"/>
   </tableColumns>
@@ -546,9 +503,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{06875460-8491-4725-9779-5103659E4525}" name="tbl_Anzahl_Kinder" displayName="tbl_Anzahl_Kinder" ref="I1:I102" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="I1:I102" xr:uid="{06875460-8491-4725-9779-5103659E4525}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{06875460-8491-4725-9779-5103659E4525}" name="tbl_Anzahl_Kinder" displayName="tbl_Anzahl_Kinder" ref="G1:G102" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="G1:G102" xr:uid="{06875460-8491-4725-9779-5103659E4525}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{CAB87FE6-84F2-445A-98E2-61DBBA398E8A}" name="Anzahl Kinder"/>
   </tableColumns>
@@ -556,9 +513,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76FD4837-88D5-472C-B63B-18AFD1F879BF}" name="Tabelle6" displayName="Tabelle6" ref="K1:K4" totalsRowShown="0">
-  <autoFilter ref="K1:K4" xr:uid="{76FD4837-88D5-472C-B63B-18AFD1F879BF}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{76FD4837-88D5-472C-B63B-18AFD1F879BF}" name="Tabelle6" displayName="Tabelle6" ref="I1:I4" totalsRowShown="0">
+  <autoFilter ref="I1:I4" xr:uid="{76FD4837-88D5-472C-B63B-18AFD1F879BF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B17BFB7B-D737-4004-A666-E7AEBE615E3C}" name="Ost/West/Ausland"/>
   </tableColumns>
@@ -831,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,7 +811,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -862,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -876,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -953,10 +910,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -985,10 +942,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1020,7 +977,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1028,7 +985,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1052,23 +1009,23 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1076,7 +1033,7 @@
         <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1084,7 +1041,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1092,7 +1049,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1100,7 +1057,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1108,52 +1065,52 @@
         <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B40" s="10">
         <v>1</v>
@@ -1164,15 +1121,15 @@
         <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1185,7 +1142,7 @@
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B44" s="4">
         <v>0</v>
@@ -1193,34 +1150,34 @@
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1238,40 +1195,34 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E880C197-BC95-4C5B-A656-6C63E902724E}">
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCDEDDF9-8147-443B-8508-A6C8D922FCA7}">
-          <x14:formula1>
-            <xm:f>Tabelle2!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B24</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7DA73FF-D468-4194-9329-301A08ACE2B5}">
           <x14:formula1>
-            <xm:f>Tabelle2!$E$2:$E$7</xm:f>
+            <xm:f>Tabelle2!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>B25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A420BD95-21E4-42A6-83BB-B7592398D91C}">
           <x14:formula1>
-            <xm:f>Tabelle2!$G$2:$G$3</xm:f>
+            <xm:f>Tabelle2!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B29 B33 B41:B42 B45:B48 B35:B39</xm:sqref>
+          <xm:sqref>B29 B38:B39 B35 B45:B48 B41:B42 B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
           <x14:formula1>
-            <xm:f>Tabelle2!$I$2:$I$102</xm:f>
+            <xm:f>Tabelle2!$G$2:$G$102</xm:f>
           </x14:formula1>
           <xm:sqref>B40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{340FCE44-5214-4D19-BA6F-DBB2AFEDFBC9}">
           <x14:formula1>
-            <xm:f>Tabelle2!$K$2:$K$4</xm:f>
+            <xm:f>Tabelle2!$I$2:$I$4</xm:f>
           </x14:formula1>
           <xm:sqref>B19</xm:sqref>
         </x14:dataValidation>
@@ -1283,615 +1234,592 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41E031-B515-4B55-B38F-F0D31894393C}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G58">
         <v>56</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G89">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G90">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G91">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I34">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I35">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I36">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I37">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I40">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I41">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I46">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I47">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I54">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I55">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I56">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I74">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I75">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I76">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I77">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I78">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I79">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I80">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I81">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I82">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I83">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I84">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I85">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I86">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I87">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I88">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I89">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I90">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I91">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I92">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I93">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I94">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I95">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I96">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I97">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G97">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I98">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G98">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I99">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G99">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I100">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G100">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I101">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G101">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I102">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G102">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="6">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>